<commit_message>
SSDM-13256: Fixed the "No value present" exception.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-with-chained-sample-properties.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-with-chained-sample-properties.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="49">
   <si>
     <t xml:space="preserve">SAMPLE_TYPE</t>
   </si>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Dynamic script</t>
   </si>
   <si>
-    <t xml:space="preserve">NAME</t>
+    <t xml:space="preserve">$NAME</t>
   </si>
   <si>
     <t xml:space="preserve">General info</t>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t xml:space="preserve">date_range_validation.py</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$NAME</t>
   </si>
   <si>
     <t xml:space="preserve">OPEN</t>
@@ -322,7 +319,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -378,7 +375,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17:G18"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -788,7 +785,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>11</v>
@@ -814,7 +811,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>11</v>
@@ -826,21 +823,21 @@
         <v>22</v>
       </c>
       <c r="E21" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>11</v>
@@ -852,21 +849,21 @@
         <v>22</v>
       </c>
       <c r="E22" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>44</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>11</v>
@@ -878,21 +875,21 @@
         <v>22</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>10</v>
@@ -904,13 +901,13 @@
         <v>22</v>
       </c>
       <c r="E24" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="H24" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>